<commit_message>
data: Correción a datos que con errores de ortografía
</commit_message>
<xml_diff>
--- a/data/processed/servicios_cult_soc_dep_rec_issste2025.xlsx
+++ b/data/processed/servicios_cult_soc_dep_rec_issste2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A67D9-C795-42E6-95E2-155F22494A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9E82C9-89FB-479C-87EE-CE481BFE43D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="60">
   <si>
     <t>Aguascalientes</t>
   </si>
   <si>
     <t>Baja California</t>
-  </si>
-  <si>
-    <t>Baja California Sur</t>
   </si>
   <si>
     <t>Campeche</t>
@@ -61,19 +58,10 @@
     <t>Jalisco</t>
   </si>
   <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Michoacan</t>
-  </si>
-  <si>
     <t>Morelos</t>
   </si>
   <si>
     <t>Nayarit</t>
-  </si>
-  <si>
-    <t>Nuevo Leon</t>
   </si>
   <si>
     <t>Oaxaca</t>
@@ -82,13 +70,7 @@
     <t>Puebla</t>
   </si>
   <si>
-    <t>Queretaro</t>
-  </si>
-  <si>
     <t>Quintana Roo</t>
-  </si>
-  <si>
-    <t>San Luis Potosi</t>
   </si>
   <si>
     <t>Sinaloa</t>
@@ -109,22 +91,7 @@
     <t>Veracruz</t>
   </si>
   <si>
-    <t>Yucatan</t>
-  </si>
-  <si>
     <t>Zacatecas</t>
-  </si>
-  <si>
-    <t>Subdeleg.Norte</t>
-  </si>
-  <si>
-    <t>Subdeleg. Sur</t>
-  </si>
-  <si>
-    <t>Subdeleg. Oriente</t>
-  </si>
-  <si>
-    <t>Subdeleg. Poniente</t>
   </si>
   <si>
     <t>Oficinas Centrales</t>
@@ -134,12 +101,6 @@
   </si>
   <si>
     <t>Issstehuixtla</t>
-  </si>
-  <si>
-    <t>Baja Calif. Norte</t>
-  </si>
-  <si>
-    <t>Baja Calif. Sur</t>
   </si>
   <si>
     <t>Regional Norte</t>
@@ -161,21 +122,6 @@
   </si>
   <si>
     <t>Baja California. Sur</t>
-  </si>
-  <si>
-    <t>Delegacion Norte</t>
-  </si>
-  <si>
-    <t>Delegacion Sur</t>
-  </si>
-  <si>
-    <t>Delegacion Oriente</t>
-  </si>
-  <si>
-    <t>Delegacion Poniente</t>
-  </si>
-  <si>
-    <t>ÃÂ¿Â½Reas Centrales</t>
   </si>
   <si>
     <t>Año</t>
@@ -209,6 +155,51 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Áreas Centrales</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>Michoacán</t>
+  </si>
+  <si>
+    <t>Nuevo León</t>
+  </si>
+  <si>
+    <t>Querétaro</t>
+  </si>
+  <si>
+    <t>San Luis Potosí</t>
+  </si>
+  <si>
+    <t>Yucatán</t>
+  </si>
+  <si>
+    <t>Delegación Norte</t>
+  </si>
+  <si>
+    <t>Delegación Sur</t>
+  </si>
+  <si>
+    <t>Delegación Oriente</t>
+  </si>
+  <si>
+    <t>Delegación Poniente</t>
+  </si>
+  <si>
+    <t>Subdelegación. Norte</t>
+  </si>
+  <si>
+    <t>Subdelegación. Sur</t>
+  </si>
+  <si>
+    <t>Subdelegación. Oriente</t>
+  </si>
+  <si>
+    <t>Subdelegación. Poniente</t>
   </si>
 </sst>
 </file>
@@ -741,27 +732,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -809,17 +780,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01004CAF-B0EE-4A4F-99F5-2C4E7F69B1DF}" name="Tabla1" displayName="Tabla1" ref="A1:K495" totalsRowShown="0">
   <autoFilter ref="A1:K495" xr:uid="{01004CAF-B0EE-4A4F-99F5-2C4E7F69B1DF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E00903E2-5B95-4A2E-B89D-5B0052D7F544}" name="Año" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{E00903E2-5B95-4A2E-B89D-5B0052D7F544}" name="Año" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{6015B546-CCE8-49F7-AD82-A56721BEB06D}" name="Oficina Representación"/>
-    <tableColumn id="3" xr3:uid="{6C24FA5D-647C-4DF8-A6EA-66A6E6528CE5}" name="Serv. Culturales Derecho Hab Publ" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{5625FA80-061B-464D-B123-C974C04DA294}" name="Serv. Deportivos Derecho Hab Publ" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{24DE0E05-24AF-4FCC-9633-B84A75B97D9A}" name="Serv. Sociales Derecho Hab Publ" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{2AC1C74A-7627-48C3-AC0B-15FBB8351EE0}" name="Serv. Funerarios Derecho Hab Publ" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{3E1E2BD6-8333-4561-B9F1-248EFBB7920E}" name="Serv. Sociales Pensionados Jubl" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{2AC1B96B-1C99-43AF-AFED-47F1F4C408FD}" name="Fome Deportivo Pensionados Jubl" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{E70B6682-15CA-4E92-BD60-818587E36A59}" name="Serv. Culturales Pensionados Jubl" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{08067B72-2814-4712-B380-BB03A667992C}" name="Soci Comedores Pensionados Jubl" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{230A8DA6-C4FF-44BE-9A39-A60006ECF43E}" name="Fecha" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{6C24FA5D-647C-4DF8-A6EA-66A6E6528CE5}" name="Serv. Culturales Derecho Hab Publ" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{5625FA80-061B-464D-B123-C974C04DA294}" name="Serv. Deportivos Derecho Hab Publ" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{24DE0E05-24AF-4FCC-9633-B84A75B97D9A}" name="Serv. Sociales Derecho Hab Publ" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{2AC1C74A-7627-48C3-AC0B-15FBB8351EE0}" name="Serv. Funerarios Derecho Hab Publ" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{3E1E2BD6-8333-4561-B9F1-248EFBB7920E}" name="Serv. Sociales Pensionados Jubl" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2AC1B96B-1C99-43AF-AFED-47F1F4C408FD}" name="Fome Deportivo Pensionados Jubl" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{E70B6682-15CA-4E92-BD60-818587E36A59}" name="Serv. Culturales Pensionados Jubl" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{08067B72-2814-4712-B380-BB03A667992C}" name="Soci Comedores Pensionados Jubl" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{230A8DA6-C4FF-44BE-9A39-A60006ECF43E}" name="Fecha" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1125,7 +1096,7 @@
   <dimension ref="A1:K495"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,37 +1116,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1253,7 +1224,7 @@
         <v>2013</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2">
         <v>22917</v>
@@ -1288,7 +1259,7 @@
         <v>2013</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2">
         <v>85376</v>
@@ -1323,7 +1294,7 @@
         <v>2013</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
         <v>65886</v>
@@ -1358,7 +1329,7 @@
         <v>2013</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2">
         <v>75766</v>
@@ -1393,7 +1364,7 @@
         <v>2013</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
         <v>92979</v>
@@ -1428,7 +1399,7 @@
         <v>2013</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
         <v>39497</v>
@@ -1463,7 +1434,7 @@
         <v>2013</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2">
         <v>88495</v>
@@ -1498,7 +1469,7 @@
         <v>2013</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2">
         <v>100270</v>
@@ -1533,7 +1504,7 @@
         <v>2013</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2">
         <v>41618</v>
@@ -1568,7 +1539,7 @@
         <v>2013</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2">
         <v>111194</v>
@@ -1603,7 +1574,7 @@
         <v>2013</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <v>43939</v>
@@ -1638,7 +1609,7 @@
         <v>2013</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2">
         <v>81763</v>
@@ -1673,7 +1644,7 @@
         <v>2013</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2">
         <v>19086</v>
@@ -1708,7 +1679,7 @@
         <v>2013</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
         <v>144600</v>
@@ -1743,7 +1714,7 @@
         <v>2013</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2">
         <v>88738</v>
@@ -1778,7 +1749,7 @@
         <v>2013</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2">
         <v>133369</v>
@@ -1813,7 +1784,7 @@
         <v>2013</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2">
         <v>273717</v>
@@ -1848,7 +1819,7 @@
         <v>2013</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2">
         <v>12395</v>
@@ -1883,7 +1854,7 @@
         <v>2013</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2">
         <v>34708</v>
@@ -1918,7 +1889,7 @@
         <v>2013</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2">
         <v>60073</v>
@@ -1953,7 +1924,7 @@
         <v>2013</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2">
         <v>163205</v>
@@ -1988,7 +1959,7 @@
         <v>2013</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C25" s="2">
         <v>50637</v>
@@ -2023,7 +1994,7 @@
         <v>2013</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" s="2">
         <v>65564</v>
@@ -2058,7 +2029,7 @@
         <v>2013</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C27" s="2">
         <v>43996</v>
@@ -2093,7 +2064,7 @@
         <v>2013</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C28" s="2">
         <v>12487</v>
@@ -2128,7 +2099,7 @@
         <v>2013</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2">
         <v>132736</v>
@@ -2163,7 +2134,7 @@
         <v>2013</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2">
         <v>40535</v>
@@ -2198,7 +2169,7 @@
         <v>2013</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C31" s="2">
         <v>115974</v>
@@ -2233,7 +2204,7 @@
         <v>2013</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2">
         <v>116532</v>
@@ -2268,7 +2239,7 @@
         <v>2013</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2">
         <v>110241</v>
@@ -2303,7 +2274,7 @@
         <v>2013</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C34" s="2">
         <v>77535</v>
@@ -2338,7 +2309,7 @@
         <v>2013</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C35" s="2">
         <v>116369</v>
@@ -2373,7 +2344,7 @@
         <v>2013</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C36" s="2">
         <v>117133</v>
@@ -2408,7 +2379,7 @@
         <v>2013</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C37" s="2">
         <v>4458940</v>
@@ -2443,7 +2414,7 @@
         <v>2013</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C38" s="2">
         <v>0</v>
@@ -2478,7 +2449,7 @@
         <v>2013</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C39" s="2">
         <v>0</v>
@@ -2583,7 +2554,7 @@
         <v>2014</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C42" s="2">
         <v>29076</v>
@@ -2618,7 +2589,7 @@
         <v>2014</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" s="2">
         <v>87248</v>
@@ -2653,7 +2624,7 @@
         <v>2014</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="2">
         <v>49368</v>
@@ -2688,7 +2659,7 @@
         <v>2014</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="2">
         <v>77475</v>
@@ -2723,7 +2694,7 @@
         <v>2014</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" s="2">
         <v>18086</v>
@@ -2758,7 +2729,7 @@
         <v>2014</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2">
         <v>92443</v>
@@ -2793,7 +2764,7 @@
         <v>2014</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="2">
         <v>62371</v>
@@ -2828,7 +2799,7 @@
         <v>2014</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="2">
         <v>55334</v>
@@ -2863,7 +2834,7 @@
         <v>2014</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2">
         <v>43644</v>
@@ -2898,7 +2869,7 @@
         <v>2014</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" s="2">
         <v>118420</v>
@@ -2933,7 +2904,7 @@
         <v>2014</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52" s="2">
         <v>50549</v>
@@ -2968,7 +2939,7 @@
         <v>2014</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C53" s="2">
         <v>244524</v>
@@ -3003,7 +2974,7 @@
         <v>2014</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C54" s="2">
         <v>116900</v>
@@ -3038,7 +3009,7 @@
         <v>2014</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C55" s="2">
         <v>128923</v>
@@ -3073,7 +3044,7 @@
         <v>2014</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C56" s="2">
         <v>90923</v>
@@ -3108,7 +3079,7 @@
         <v>2014</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C57" s="2">
         <v>106619</v>
@@ -3143,7 +3114,7 @@
         <v>2014</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C58" s="2">
         <v>279230</v>
@@ -3178,7 +3149,7 @@
         <v>2014</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C59" s="2">
         <v>54049</v>
@@ -3213,7 +3184,7 @@
         <v>2014</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C60" s="2">
         <v>41550</v>
@@ -3248,7 +3219,7 @@
         <v>2014</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C61" s="2">
         <v>11174</v>
@@ -3283,7 +3254,7 @@
         <v>2014</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C62" s="2">
         <v>209668</v>
@@ -3318,7 +3289,7 @@
         <v>2014</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C63" s="2">
         <v>32266</v>
@@ -3353,7 +3324,7 @@
         <v>2014</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C64" s="2">
         <v>68395</v>
@@ -3388,7 +3359,7 @@
         <v>2014</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C65" s="2">
         <v>56276</v>
@@ -3423,7 +3394,7 @@
         <v>2014</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C66" s="2">
         <v>21459</v>
@@ -3458,7 +3429,7 @@
         <v>2014</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C67" s="2">
         <v>108344</v>
@@ -3493,7 +3464,7 @@
         <v>2014</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C68" s="2">
         <v>57523</v>
@@ -3528,7 +3499,7 @@
         <v>2014</v>
       </c>
       <c r="B69" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C69" s="2">
         <v>136792</v>
@@ -3563,7 +3534,7 @@
         <v>2014</v>
       </c>
       <c r="B70" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C70" s="2">
         <v>120190</v>
@@ -3598,7 +3569,7 @@
         <v>2014</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C71" s="2">
         <v>101457</v>
@@ -3633,7 +3604,7 @@
         <v>2014</v>
       </c>
       <c r="B72" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C72" s="2">
         <v>88242</v>
@@ -3668,7 +3639,7 @@
         <v>2014</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C73" s="2">
         <v>91827</v>
@@ -3703,7 +3674,7 @@
         <v>2014</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C74" s="2">
         <v>154188</v>
@@ -3738,7 +3709,7 @@
         <v>2014</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C75" s="2">
         <v>2893725</v>
@@ -3773,7 +3744,7 @@
         <v>2014</v>
       </c>
       <c r="B76" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
@@ -3808,7 +3779,7 @@
         <v>2014</v>
       </c>
       <c r="B77" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -3913,7 +3884,7 @@
         <v>2015</v>
       </c>
       <c r="B80" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C80" s="2">
         <v>25967</v>
@@ -3948,7 +3919,7 @@
         <v>2015</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81" s="2">
         <v>74323</v>
@@ -3983,7 +3954,7 @@
         <v>2015</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C82" s="2">
         <v>59386</v>
@@ -4018,7 +3989,7 @@
         <v>2015</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C83" s="2">
         <v>69174</v>
@@ -4053,7 +4024,7 @@
         <v>2015</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C84" s="2">
         <v>36710</v>
@@ -4088,7 +4059,7 @@
         <v>2015</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C85" s="2">
         <v>77265</v>
@@ -4123,7 +4094,7 @@
         <v>2015</v>
       </c>
       <c r="B86" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C86" s="2">
         <v>83066</v>
@@ -4158,7 +4129,7 @@
         <v>2015</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C87" s="2">
         <v>33575</v>
@@ -4193,7 +4164,7 @@
         <v>2015</v>
       </c>
       <c r="B88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C88" s="2">
         <v>39556</v>
@@ -4228,7 +4199,7 @@
         <v>2015</v>
       </c>
       <c r="B89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C89" s="2">
         <v>106996</v>
@@ -4263,7 +4234,7 @@
         <v>2015</v>
       </c>
       <c r="B90" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C90" s="2">
         <v>48617</v>
@@ -4298,7 +4269,7 @@
         <v>2015</v>
       </c>
       <c r="B91" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C91" s="2">
         <v>243748</v>
@@ -4333,7 +4304,7 @@
         <v>2015</v>
       </c>
       <c r="B92" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C92" s="2">
         <v>67161</v>
@@ -4368,7 +4339,7 @@
         <v>2015</v>
       </c>
       <c r="B93" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C93" s="2">
         <v>117939</v>
@@ -4403,7 +4374,7 @@
         <v>2015</v>
       </c>
       <c r="B94" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C94" s="2">
         <v>86309</v>
@@ -4438,7 +4409,7 @@
         <v>2015</v>
       </c>
       <c r="B95" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C95" s="2">
         <v>114666</v>
@@ -4473,7 +4444,7 @@
         <v>2015</v>
       </c>
       <c r="B96" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C96" s="2">
         <v>279410</v>
@@ -4508,7 +4479,7 @@
         <v>2015</v>
       </c>
       <c r="B97" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C97" s="2">
         <v>74815</v>
@@ -4543,7 +4514,7 @@
         <v>2015</v>
       </c>
       <c r="B98" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C98" s="2">
         <v>38881</v>
@@ -4578,7 +4549,7 @@
         <v>2015</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C99" s="2">
         <v>13941</v>
@@ -4613,7 +4584,7 @@
         <v>2015</v>
       </c>
       <c r="B100" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C100" s="2">
         <v>234704</v>
@@ -4648,7 +4619,7 @@
         <v>2015</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C101" s="2">
         <v>47451</v>
@@ -4683,7 +4654,7 @@
         <v>2015</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C102" s="2">
         <v>61553</v>
@@ -4718,7 +4689,7 @@
         <v>2015</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C103" s="2">
         <v>63340</v>
@@ -4753,7 +4724,7 @@
         <v>2015</v>
       </c>
       <c r="B104" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C104" s="2">
         <v>32266</v>
@@ -4788,7 +4759,7 @@
         <v>2015</v>
       </c>
       <c r="B105" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C105" s="2">
         <v>113562</v>
@@ -4823,7 +4794,7 @@
         <v>2015</v>
       </c>
       <c r="B106" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C106" s="2">
         <v>59809</v>
@@ -4858,7 +4829,7 @@
         <v>2015</v>
       </c>
       <c r="B107" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C107" s="2">
         <v>137489</v>
@@ -4893,7 +4864,7 @@
         <v>2015</v>
       </c>
       <c r="B108" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C108" s="2">
         <v>119575</v>
@@ -4928,7 +4899,7 @@
         <v>2015</v>
       </c>
       <c r="B109" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C109" s="2">
         <v>91117</v>
@@ -4963,7 +4934,7 @@
         <v>2015</v>
       </c>
       <c r="B110" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C110" s="2">
         <v>187915</v>
@@ -4998,7 +4969,7 @@
         <v>2015</v>
       </c>
       <c r="B111" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C111" s="2">
         <v>67770</v>
@@ -5033,7 +5004,7 @@
         <v>2015</v>
       </c>
       <c r="B112" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C112" s="2">
         <v>113765</v>
@@ -5068,7 +5039,7 @@
         <v>2015</v>
       </c>
       <c r="B113" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C113" s="2">
         <v>2730808</v>
@@ -5103,7 +5074,7 @@
         <v>2015</v>
       </c>
       <c r="B114" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
@@ -5138,7 +5109,7 @@
         <v>2015</v>
       </c>
       <c r="B115" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C115" s="2">
         <v>0</v>
@@ -5208,7 +5179,7 @@
         <v>2016</v>
       </c>
       <c r="B117" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C117" s="2">
         <v>60463</v>
@@ -5243,7 +5214,7 @@
         <v>2016</v>
       </c>
       <c r="B118" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C118" s="2">
         <v>10646</v>
@@ -5278,7 +5249,7 @@
         <v>2016</v>
       </c>
       <c r="B119" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C119" s="2">
         <v>66560</v>
@@ -5313,7 +5284,7 @@
         <v>2016</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120" s="2">
         <v>50498</v>
@@ -5348,7 +5319,7 @@
         <v>2016</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C121" s="2">
         <v>47575</v>
@@ -5383,7 +5354,7 @@
         <v>2016</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C122" s="2">
         <v>42348</v>
@@ -5418,7 +5389,7 @@
         <v>2016</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C123" s="2">
         <v>55337</v>
@@ -5453,7 +5424,7 @@
         <v>2016</v>
       </c>
       <c r="B124" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C124" s="2">
         <v>54284</v>
@@ -5488,7 +5459,7 @@
         <v>2016</v>
       </c>
       <c r="B125" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C125" s="2">
         <v>39484</v>
@@ -5523,7 +5494,7 @@
         <v>2016</v>
       </c>
       <c r="B126" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C126" s="2">
         <v>24074</v>
@@ -5558,7 +5529,7 @@
         <v>2016</v>
       </c>
       <c r="B127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C127" s="2">
         <v>81480</v>
@@ -5593,7 +5564,7 @@
         <v>2016</v>
       </c>
       <c r="B128" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C128" s="2">
         <v>106131</v>
@@ -5628,7 +5599,7 @@
         <v>2016</v>
       </c>
       <c r="B129" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C129" s="2">
         <v>176504</v>
@@ -5663,7 +5634,7 @@
         <v>2016</v>
       </c>
       <c r="B130" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C130" s="2">
         <v>26285</v>
@@ -5698,7 +5669,7 @@
         <v>2016</v>
       </c>
       <c r="B131" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C131" s="2">
         <v>90000</v>
@@ -5733,7 +5704,7 @@
         <v>2016</v>
       </c>
       <c r="B132" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C132" s="2">
         <v>54231</v>
@@ -5768,7 +5739,7 @@
         <v>2016</v>
       </c>
       <c r="B133" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C133" s="2">
         <v>87877</v>
@@ -5803,7 +5774,7 @@
         <v>2016</v>
       </c>
       <c r="B134" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C134" s="2">
         <v>203286</v>
@@ -5838,7 +5809,7 @@
         <v>2016</v>
       </c>
       <c r="B135" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C135" s="2">
         <v>62651</v>
@@ -5873,7 +5844,7 @@
         <v>2016</v>
       </c>
       <c r="B136" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C136" s="2">
         <v>39760</v>
@@ -5908,7 +5879,7 @@
         <v>2016</v>
       </c>
       <c r="B137" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C137" s="2">
         <v>8331</v>
@@ -5943,7 +5914,7 @@
         <v>2016</v>
       </c>
       <c r="B138" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C138" s="2">
         <v>162819</v>
@@ -5978,7 +5949,7 @@
         <v>2016</v>
       </c>
       <c r="B139" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C139" s="2">
         <v>46584</v>
@@ -6013,7 +5984,7 @@
         <v>2016</v>
       </c>
       <c r="B140" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C140" s="2">
         <v>75593</v>
@@ -6048,7 +6019,7 @@
         <v>2016</v>
       </c>
       <c r="B141" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C141" s="2">
         <v>59027</v>
@@ -6083,7 +6054,7 @@
         <v>2016</v>
       </c>
       <c r="B142" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C142" s="2">
         <v>16579</v>
@@ -6118,7 +6089,7 @@
         <v>2016</v>
       </c>
       <c r="B143" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C143" s="2">
         <v>85891</v>
@@ -6153,7 +6124,7 @@
         <v>2016</v>
       </c>
       <c r="B144" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C144" s="2">
         <v>50857</v>
@@ -6188,7 +6159,7 @@
         <v>2016</v>
       </c>
       <c r="B145" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C145" s="2">
         <v>92295</v>
@@ -6223,7 +6194,7 @@
         <v>2016</v>
       </c>
       <c r="B146" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C146" s="2">
         <v>90445</v>
@@ -6258,7 +6229,7 @@
         <v>2016</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C147" s="2">
         <v>84266</v>
@@ -6293,7 +6264,7 @@
         <v>2016</v>
       </c>
       <c r="B148" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C148" s="2">
         <v>145297</v>
@@ -6328,7 +6299,7 @@
         <v>2016</v>
       </c>
       <c r="B149" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C149" s="2">
         <v>21249</v>
@@ -6363,7 +6334,7 @@
         <v>2016</v>
       </c>
       <c r="B150" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C150" s="2">
         <v>103051</v>
@@ -6398,7 +6369,7 @@
         <v>2016</v>
       </c>
       <c r="B151" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C151" s="2">
         <v>972448</v>
@@ -6433,7 +6404,7 @@
         <v>2016</v>
       </c>
       <c r="B152" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -6468,7 +6439,7 @@
         <v>2016</v>
       </c>
       <c r="B153" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6538,7 +6509,7 @@
         <v>2017</v>
       </c>
       <c r="B155" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C155" s="2">
         <v>68545</v>
@@ -6573,7 +6544,7 @@
         <v>2017</v>
       </c>
       <c r="B156" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C156" s="2">
         <v>17482</v>
@@ -6608,7 +6579,7 @@
         <v>2017</v>
       </c>
       <c r="B157" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C157" s="2">
         <v>76202</v>
@@ -6643,7 +6614,7 @@
         <v>2017</v>
       </c>
       <c r="B158" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C158" s="2">
         <v>75566</v>
@@ -6678,7 +6649,7 @@
         <v>2017</v>
       </c>
       <c r="B159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C159" s="2">
         <v>68319</v>
@@ -6713,7 +6684,7 @@
         <v>2017</v>
       </c>
       <c r="B160" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C160" s="2">
         <v>80363</v>
@@ -6748,7 +6719,7 @@
         <v>2017</v>
       </c>
       <c r="B161" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C161" s="2">
         <v>79465</v>
@@ -6783,7 +6754,7 @@
         <v>2017</v>
       </c>
       <c r="B162" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C162" s="2">
         <v>89897</v>
@@ -6818,7 +6789,7 @@
         <v>2017</v>
       </c>
       <c r="B163" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C163" s="2">
         <v>45528</v>
@@ -6853,7 +6824,7 @@
         <v>2017</v>
       </c>
       <c r="B164" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C164" s="2">
         <v>37993</v>
@@ -6888,7 +6859,7 @@
         <v>2017</v>
       </c>
       <c r="B165" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C165" s="2">
         <v>121807</v>
@@ -6923,7 +6894,7 @@
         <v>2017</v>
       </c>
       <c r="B166" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C166" s="2">
         <v>109999</v>
@@ -6958,7 +6929,7 @@
         <v>2017</v>
       </c>
       <c r="B167" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C167" s="2">
         <v>236567</v>
@@ -6993,7 +6964,7 @@
         <v>2017</v>
       </c>
       <c r="B168" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C168" s="2">
         <v>67230</v>
@@ -7028,7 +6999,7 @@
         <v>2017</v>
       </c>
       <c r="B169" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C169" s="2">
         <v>81174</v>
@@ -7063,7 +7034,7 @@
         <v>2017</v>
       </c>
       <c r="B170" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C170" s="2">
         <v>46665</v>
@@ -7098,7 +7069,7 @@
         <v>2017</v>
       </c>
       <c r="B171" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C171" s="2">
         <v>108205</v>
@@ -7133,7 +7104,7 @@
         <v>2017</v>
       </c>
       <c r="B172" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C172" s="2">
         <v>278566</v>
@@ -7168,7 +7139,7 @@
         <v>2017</v>
       </c>
       <c r="B173" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C173" s="2">
         <v>82972</v>
@@ -7203,7 +7174,7 @@
         <v>2017</v>
       </c>
       <c r="B174" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C174" s="2">
         <v>51946</v>
@@ -7238,7 +7209,7 @@
         <v>2017</v>
       </c>
       <c r="B175" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C175" s="2">
         <v>35766</v>
@@ -7273,7 +7244,7 @@
         <v>2017</v>
       </c>
       <c r="B176" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C176" s="2">
         <v>184992</v>
@@ -7308,7 +7279,7 @@
         <v>2017</v>
       </c>
       <c r="B177" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C177" s="2">
         <v>67339</v>
@@ -7343,7 +7314,7 @@
         <v>2017</v>
       </c>
       <c r="B178" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C178" s="2">
         <v>100728</v>
@@ -7378,7 +7349,7 @@
         <v>2017</v>
       </c>
       <c r="B179" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C179" s="2">
         <v>101825</v>
@@ -7413,7 +7384,7 @@
         <v>2017</v>
       </c>
       <c r="B180" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C180" s="2">
         <v>22121</v>
@@ -7448,7 +7419,7 @@
         <v>2017</v>
       </c>
       <c r="B181" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C181" s="2">
         <v>95061</v>
@@ -7483,7 +7454,7 @@
         <v>2017</v>
       </c>
       <c r="B182" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C182" s="2">
         <v>70079</v>
@@ -7518,7 +7489,7 @@
         <v>2017</v>
       </c>
       <c r="B183" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C183" s="2">
         <v>107583</v>
@@ -7553,7 +7524,7 @@
         <v>2017</v>
       </c>
       <c r="B184" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C184" s="2">
         <v>121744</v>
@@ -7588,7 +7559,7 @@
         <v>2017</v>
       </c>
       <c r="B185" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C185" s="2">
         <v>145522</v>
@@ -7623,7 +7594,7 @@
         <v>2017</v>
       </c>
       <c r="B186" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C186" s="2">
         <v>85815</v>
@@ -7658,7 +7629,7 @@
         <v>2017</v>
       </c>
       <c r="B187" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C187" s="2">
         <v>34875</v>
@@ -7693,7 +7664,7 @@
         <v>2017</v>
       </c>
       <c r="B188" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C188" s="2">
         <v>151018</v>
@@ -7728,7 +7699,7 @@
         <v>2017</v>
       </c>
       <c r="B189" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C189" s="2">
         <v>1138040</v>
@@ -7763,7 +7734,7 @@
         <v>2017</v>
       </c>
       <c r="B190" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7798,7 +7769,7 @@
         <v>2017</v>
       </c>
       <c r="B191" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7868,7 +7839,7 @@
         <v>2018</v>
       </c>
       <c r="B193" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C193" s="2">
         <v>67147</v>
@@ -7903,7 +7874,7 @@
         <v>2018</v>
       </c>
       <c r="B194" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C194" s="2">
         <v>13774</v>
@@ -7938,7 +7909,7 @@
         <v>2018</v>
       </c>
       <c r="B195" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C195" s="2">
         <v>57071</v>
@@ -7973,7 +7944,7 @@
         <v>2018</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C196" s="2">
         <v>79543</v>
@@ -8008,7 +7979,7 @@
         <v>2018</v>
       </c>
       <c r="B197" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C197" s="2">
         <v>67456</v>
@@ -8043,7 +8014,7 @@
         <v>2018</v>
       </c>
       <c r="B198" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C198" s="2">
         <v>58020</v>
@@ -8078,7 +8049,7 @@
         <v>2018</v>
       </c>
       <c r="B199" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C199" s="2">
         <v>54085</v>
@@ -8113,7 +8084,7 @@
         <v>2018</v>
       </c>
       <c r="B200" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C200" s="2">
         <v>98725</v>
@@ -8148,7 +8119,7 @@
         <v>2018</v>
       </c>
       <c r="B201" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C201" s="2">
         <v>37452</v>
@@ -8183,7 +8154,7 @@
         <v>2018</v>
       </c>
       <c r="B202" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C202" s="2">
         <v>37752</v>
@@ -8218,7 +8189,7 @@
         <v>2018</v>
       </c>
       <c r="B203" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C203" s="2">
         <v>140786</v>
@@ -8253,7 +8224,7 @@
         <v>2018</v>
       </c>
       <c r="B204" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C204" s="2">
         <v>107142</v>
@@ -8288,7 +8259,7 @@
         <v>2018</v>
       </c>
       <c r="B205" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C205" s="2">
         <v>240729</v>
@@ -8323,7 +8294,7 @@
         <v>2018</v>
       </c>
       <c r="B206" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C206" s="2">
         <v>50676</v>
@@ -8358,7 +8329,7 @@
         <v>2018</v>
       </c>
       <c r="B207" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C207" s="2">
         <v>84731</v>
@@ -8393,7 +8364,7 @@
         <v>2018</v>
       </c>
       <c r="B208" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C208" s="2">
         <v>50722</v>
@@ -8428,7 +8399,7 @@
         <v>2018</v>
       </c>
       <c r="B209" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C209" s="2">
         <v>99373</v>
@@ -8463,7 +8434,7 @@
         <v>2018</v>
       </c>
       <c r="B210" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C210" s="2">
         <v>275284</v>
@@ -8498,7 +8469,7 @@
         <v>2018</v>
       </c>
       <c r="B211" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C211" s="2">
         <v>81969</v>
@@ -8533,7 +8504,7 @@
         <v>2018</v>
       </c>
       <c r="B212" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C212" s="2">
         <v>55687</v>
@@ -8568,7 +8539,7 @@
         <v>2018</v>
       </c>
       <c r="B213" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C213" s="2">
         <v>20901</v>
@@ -8603,7 +8574,7 @@
         <v>2018</v>
       </c>
       <c r="B214" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C214" s="2">
         <v>196588</v>
@@ -8638,7 +8609,7 @@
         <v>2018</v>
       </c>
       <c r="B215" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C215" s="2">
         <v>67576</v>
@@ -8673,7 +8644,7 @@
         <v>2018</v>
       </c>
       <c r="B216" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C216" s="2">
         <v>104609</v>
@@ -8708,7 +8679,7 @@
         <v>2018</v>
       </c>
       <c r="B217" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C217" s="2">
         <v>116693</v>
@@ -8743,7 +8714,7 @@
         <v>2018</v>
       </c>
       <c r="B218" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C218" s="2">
         <v>23349</v>
@@ -8778,7 +8749,7 @@
         <v>2018</v>
       </c>
       <c r="B219" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C219" s="2">
         <v>99287</v>
@@ -8813,7 +8784,7 @@
         <v>2018</v>
       </c>
       <c r="B220" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C220" s="2">
         <v>62324</v>
@@ -8848,7 +8819,7 @@
         <v>2018</v>
       </c>
       <c r="B221" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C221" s="2">
         <v>93107</v>
@@ -8883,7 +8854,7 @@
         <v>2018</v>
       </c>
       <c r="B222" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C222" s="2">
         <v>121960</v>
@@ -8918,7 +8889,7 @@
         <v>2018</v>
       </c>
       <c r="B223" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C223" s="2">
         <v>132860</v>
@@ -8953,7 +8924,7 @@
         <v>2018</v>
       </c>
       <c r="B224" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C224" s="2">
         <v>66922</v>
@@ -8988,7 +8959,7 @@
         <v>2018</v>
       </c>
       <c r="B225" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C225" s="2">
         <v>38482</v>
@@ -9023,7 +8994,7 @@
         <v>2018</v>
       </c>
       <c r="B226" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C226" s="2">
         <v>142850</v>
@@ -9058,7 +9029,7 @@
         <v>2018</v>
       </c>
       <c r="B227" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C227" s="2">
         <v>1878886</v>
@@ -9093,7 +9064,7 @@
         <v>2018</v>
       </c>
       <c r="B228" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C228" s="2">
         <v>0</v>
@@ -9128,7 +9099,7 @@
         <v>2018</v>
       </c>
       <c r="B229" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C229" s="2">
         <v>0</v>
@@ -9198,7 +9169,7 @@
         <v>2019</v>
       </c>
       <c r="B231" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C231" s="2">
         <v>23337</v>
@@ -9233,7 +9204,7 @@
         <v>2019</v>
       </c>
       <c r="B232" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C232" s="2">
         <v>2923</v>
@@ -9268,7 +9239,7 @@
         <v>2019</v>
       </c>
       <c r="B233" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C233" s="2">
         <v>55339</v>
@@ -9303,7 +9274,7 @@
         <v>2019</v>
       </c>
       <c r="B234" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C234" s="2">
         <v>80616</v>
@@ -9338,7 +9309,7 @@
         <v>2019</v>
       </c>
       <c r="B235" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C235" s="2">
         <v>69491</v>
@@ -9373,7 +9344,7 @@
         <v>2019</v>
       </c>
       <c r="B236" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C236" s="2">
         <v>68503</v>
@@ -9408,7 +9379,7 @@
         <v>2019</v>
       </c>
       <c r="B237" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C237" s="2">
         <v>68938</v>
@@ -9443,7 +9414,7 @@
         <v>2019</v>
       </c>
       <c r="B238" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C238" s="2">
         <v>100926</v>
@@ -9478,7 +9449,7 @@
         <v>2019</v>
       </c>
       <c r="B239" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C239" s="2">
         <v>56113</v>
@@ -9513,7 +9484,7 @@
         <v>2019</v>
       </c>
       <c r="B240" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C240" s="2">
         <v>41697</v>
@@ -9548,7 +9519,7 @@
         <v>2019</v>
       </c>
       <c r="B241" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C241" s="2">
         <v>130797</v>
@@ -9583,7 +9554,7 @@
         <v>2019</v>
       </c>
       <c r="B242" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C242" s="2">
         <v>86896</v>
@@ -9618,7 +9589,7 @@
         <v>2019</v>
       </c>
       <c r="B243" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C243" s="2">
         <v>205948</v>
@@ -9653,7 +9624,7 @@
         <v>2019</v>
       </c>
       <c r="B244" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C244" s="2">
         <v>159861</v>
@@ -9688,7 +9659,7 @@
         <v>2019</v>
       </c>
       <c r="B245" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C245" s="2">
         <v>79641</v>
@@ -9723,7 +9694,7 @@
         <v>2019</v>
       </c>
       <c r="B246" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C246" s="2">
         <v>72968</v>
@@ -9758,7 +9729,7 @@
         <v>2019</v>
       </c>
       <c r="B247" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C247" s="2">
         <v>98414</v>
@@ -9793,7 +9764,7 @@
         <v>2019</v>
       </c>
       <c r="B248" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C248" s="2">
         <v>277218</v>
@@ -9828,7 +9799,7 @@
         <v>2019</v>
       </c>
       <c r="B249" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C249" s="2">
         <v>84659</v>
@@ -9863,7 +9834,7 @@
         <v>2019</v>
       </c>
       <c r="B250" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C250" s="2">
         <v>34865</v>
@@ -9898,7 +9869,7 @@
         <v>2019</v>
       </c>
       <c r="B251" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C251" s="2">
         <v>20761</v>
@@ -9933,7 +9904,7 @@
         <v>2019</v>
       </c>
       <c r="B252" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C252" s="2">
         <v>204535</v>
@@ -9968,7 +9939,7 @@
         <v>2019</v>
       </c>
       <c r="B253" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C253" s="2">
         <v>66325</v>
@@ -10003,7 +9974,7 @@
         <v>2019</v>
       </c>
       <c r="B254" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C254" s="2">
         <v>69680</v>
@@ -10038,7 +10009,7 @@
         <v>2019</v>
       </c>
       <c r="B255" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C255" s="2">
         <v>92025</v>
@@ -10073,7 +10044,7 @@
         <v>2019</v>
       </c>
       <c r="B256" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C256" s="2">
         <v>24855</v>
@@ -10108,7 +10079,7 @@
         <v>2019</v>
       </c>
       <c r="B257" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C257" s="2">
         <v>35401</v>
@@ -10143,7 +10114,7 @@
         <v>2019</v>
       </c>
       <c r="B258" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C258" s="2">
         <v>55111</v>
@@ -10178,7 +10149,7 @@
         <v>2019</v>
       </c>
       <c r="B259" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C259" s="2">
         <v>64862</v>
@@ -10213,7 +10184,7 @@
         <v>2019</v>
       </c>
       <c r="B260" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C260" s="2">
         <v>123350</v>
@@ -10248,7 +10219,7 @@
         <v>2019</v>
       </c>
       <c r="B261" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C261" s="2">
         <v>127697</v>
@@ -10283,7 +10254,7 @@
         <v>2019</v>
       </c>
       <c r="B262" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C262" s="2">
         <v>119571</v>
@@ -10318,7 +10289,7 @@
         <v>2019</v>
       </c>
       <c r="B263" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C263" s="2">
         <v>25401</v>
@@ -10353,7 +10324,7 @@
         <v>2019</v>
       </c>
       <c r="B264" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C264" s="2">
         <v>141741</v>
@@ -10388,7 +10359,7 @@
         <v>2019</v>
       </c>
       <c r="B265" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C265" s="2">
         <v>997716</v>
@@ -10423,7 +10394,7 @@
         <v>2019</v>
       </c>
       <c r="B266" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C266" s="2">
         <v>0</v>
@@ -10458,7 +10429,7 @@
         <v>2019</v>
       </c>
       <c r="B267" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C267" s="2">
         <v>0</v>
@@ -10528,7 +10499,7 @@
         <v>2020</v>
       </c>
       <c r="B269" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C269" s="2">
         <v>2436</v>
@@ -10563,7 +10534,7 @@
         <v>2020</v>
       </c>
       <c r="B270" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C270" s="2">
         <v>256</v>
@@ -10598,7 +10569,7 @@
         <v>2020</v>
       </c>
       <c r="B271" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C271" s="2">
         <v>23409</v>
@@ -10633,7 +10604,7 @@
         <v>2020</v>
       </c>
       <c r="B272" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C272" s="2">
         <v>12605</v>
@@ -10668,7 +10639,7 @@
         <v>2020</v>
       </c>
       <c r="B273" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C273" s="2">
         <v>0</v>
@@ -10703,7 +10674,7 @@
         <v>2020</v>
       </c>
       <c r="B274" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C274" s="2">
         <v>11790</v>
@@ -10738,7 +10709,7 @@
         <v>2020</v>
       </c>
       <c r="B275" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C275" s="2">
         <v>8471</v>
@@ -10773,7 +10744,7 @@
         <v>2020</v>
       </c>
       <c r="B276" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C276" s="2">
         <v>7777</v>
@@ -10808,7 +10779,7 @@
         <v>2020</v>
       </c>
       <c r="B277" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C277" s="2">
         <v>347</v>
@@ -10843,7 +10814,7 @@
         <v>2020</v>
       </c>
       <c r="B278" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C278" s="2">
         <v>3320</v>
@@ -10878,7 +10849,7 @@
         <v>2020</v>
       </c>
       <c r="B279" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C279" s="2">
         <v>27129</v>
@@ -10913,7 +10884,7 @@
         <v>2020</v>
       </c>
       <c r="B280" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C280" s="2">
         <v>1393</v>
@@ -10948,7 +10919,7 @@
         <v>2020</v>
       </c>
       <c r="B281" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C281" s="2">
         <v>17835</v>
@@ -10983,7 +10954,7 @@
         <v>2020</v>
       </c>
       <c r="B282" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C282" s="2">
         <v>15319</v>
@@ -11018,7 +10989,7 @@
         <v>2020</v>
       </c>
       <c r="B283" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C283" s="2">
         <v>8048</v>
@@ -11053,7 +11024,7 @@
         <v>2020</v>
       </c>
       <c r="B284" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C284" s="2">
         <v>4831</v>
@@ -11088,7 +11059,7 @@
         <v>2020</v>
       </c>
       <c r="B285" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C285" s="2">
         <v>4574</v>
@@ -11123,7 +11094,7 @@
         <v>2020</v>
       </c>
       <c r="B286" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C286" s="2">
         <v>31523</v>
@@ -11158,7 +11129,7 @@
         <v>2020</v>
       </c>
       <c r="B287" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C287" s="2">
         <v>6925</v>
@@ -11193,7 +11164,7 @@
         <v>2020</v>
       </c>
       <c r="B288" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C288" s="2">
         <v>1164</v>
@@ -11228,7 +11199,7 @@
         <v>2020</v>
       </c>
       <c r="B289" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C289" s="2">
         <v>2703</v>
@@ -11263,7 +11234,7 @@
         <v>2020</v>
       </c>
       <c r="B290" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C290" s="2">
         <v>9400</v>
@@ -11298,7 +11269,7 @@
         <v>2020</v>
       </c>
       <c r="B291" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C291" s="2">
         <v>103</v>
@@ -11333,7 +11304,7 @@
         <v>2020</v>
       </c>
       <c r="B292" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C292" s="2">
         <v>1295</v>
@@ -11368,7 +11339,7 @@
         <v>2020</v>
       </c>
       <c r="B293" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C293" s="2">
         <v>705</v>
@@ -11403,7 +11374,7 @@
         <v>2020</v>
       </c>
       <c r="B294" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C294" s="2">
         <v>3899</v>
@@ -11438,7 +11409,7 @@
         <v>2020</v>
       </c>
       <c r="B295" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C295" s="2">
         <v>10049</v>
@@ -11473,7 +11444,7 @@
         <v>2020</v>
       </c>
       <c r="B296" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C296" s="2">
         <v>7673</v>
@@ -11508,7 +11479,7 @@
         <v>2020</v>
       </c>
       <c r="B297" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C297" s="2">
         <v>10930</v>
@@ -11543,7 +11514,7 @@
         <v>2020</v>
       </c>
       <c r="B298" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C298" s="2">
         <v>12471</v>
@@ -11578,7 +11549,7 @@
         <v>2020</v>
       </c>
       <c r="B299" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C299" s="2">
         <v>16253</v>
@@ -11613,7 +11584,7 @@
         <v>2020</v>
       </c>
       <c r="B300" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C300" s="2">
         <v>11157</v>
@@ -11648,7 +11619,7 @@
         <v>2020</v>
       </c>
       <c r="B301" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C301" s="2">
         <v>158</v>
@@ -11683,7 +11654,7 @@
         <v>2020</v>
       </c>
       <c r="B302" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C302" s="2">
         <v>17236</v>
@@ -11718,7 +11689,7 @@
         <v>2020</v>
       </c>
       <c r="B303" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C303" s="2">
         <v>148392</v>
@@ -11753,7 +11724,7 @@
         <v>2020</v>
       </c>
       <c r="B304" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C304" s="2">
         <v>0</v>
@@ -11788,7 +11759,7 @@
         <v>2020</v>
       </c>
       <c r="B305" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C305" s="2">
         <v>0</v>
@@ -11858,7 +11829,7 @@
         <v>2021</v>
       </c>
       <c r="B307" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C307" s="2">
         <v>79</v>
@@ -11893,7 +11864,7 @@
         <v>2021</v>
       </c>
       <c r="B308" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C308" s="2">
         <v>9</v>
@@ -11928,7 +11899,7 @@
         <v>2021</v>
       </c>
       <c r="B309" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C309" s="2">
         <v>13</v>
@@ -11963,7 +11934,7 @@
         <v>2021</v>
       </c>
       <c r="B310" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C310" s="2">
         <v>34</v>
@@ -11998,7 +11969,7 @@
         <v>2021</v>
       </c>
       <c r="B311" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C311" s="2">
         <v>97</v>
@@ -12033,7 +12004,7 @@
         <v>2021</v>
       </c>
       <c r="B312" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C312" s="2">
         <v>254</v>
@@ -12068,7 +12039,7 @@
         <v>2021</v>
       </c>
       <c r="B313" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C313" s="2">
         <v>116</v>
@@ -12103,7 +12074,7 @@
         <v>2021</v>
       </c>
       <c r="B314" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C314" s="2">
         <v>282</v>
@@ -12138,7 +12109,7 @@
         <v>2021</v>
       </c>
       <c r="B315" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C315" s="2">
         <v>396</v>
@@ -12173,7 +12144,7 @@
         <v>2021</v>
       </c>
       <c r="B316" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C316" s="2">
         <v>139</v>
@@ -12208,7 +12179,7 @@
         <v>2021</v>
       </c>
       <c r="B317" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C317" s="2">
         <v>0</v>
@@ -12243,7 +12214,7 @@
         <v>2021</v>
       </c>
       <c r="B318" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C318" s="2">
         <v>208</v>
@@ -12278,7 +12249,7 @@
         <v>2021</v>
       </c>
       <c r="B319" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C319" s="2">
         <v>245</v>
@@ -12313,7 +12284,7 @@
         <v>2021</v>
       </c>
       <c r="B320" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C320" s="2">
         <v>830</v>
@@ -12348,7 +12319,7 @@
         <v>2021</v>
       </c>
       <c r="B321" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C321" s="2">
         <v>603</v>
@@ -12383,7 +12354,7 @@
         <v>2021</v>
       </c>
       <c r="B322" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C322" s="2">
         <v>366</v>
@@ -12418,7 +12389,7 @@
         <v>2021</v>
       </c>
       <c r="B323" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C323" s="2">
         <v>50</v>
@@ -12453,7 +12424,7 @@
         <v>2021</v>
       </c>
       <c r="B324" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C324" s="2">
         <v>269</v>
@@ -12488,7 +12459,7 @@
         <v>2021</v>
       </c>
       <c r="B325" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C325" s="2">
         <v>109</v>
@@ -12523,7 +12494,7 @@
         <v>2021</v>
       </c>
       <c r="B326" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C326" s="2">
         <v>11</v>
@@ -12558,7 +12529,7 @@
         <v>2021</v>
       </c>
       <c r="B327" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C327" s="2">
         <v>110</v>
@@ -12593,7 +12564,7 @@
         <v>2021</v>
       </c>
       <c r="B328" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C328" s="2">
         <v>145</v>
@@ -12628,7 +12599,7 @@
         <v>2021</v>
       </c>
       <c r="B329" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C329" s="2">
         <v>40</v>
@@ -12663,7 +12634,7 @@
         <v>2021</v>
       </c>
       <c r="B330" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C330" s="2">
         <v>0</v>
@@ -12698,7 +12669,7 @@
         <v>2021</v>
       </c>
       <c r="B331" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C331" s="2">
         <v>113</v>
@@ -12733,7 +12704,7 @@
         <v>2021</v>
       </c>
       <c r="B332" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C332" s="2">
         <v>19</v>
@@ -12768,7 +12739,7 @@
         <v>2021</v>
       </c>
       <c r="B333" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C333" s="2">
         <v>639</v>
@@ -12803,7 +12774,7 @@
         <v>2021</v>
       </c>
       <c r="B334" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C334" s="2">
         <v>469</v>
@@ -12838,7 +12809,7 @@
         <v>2021</v>
       </c>
       <c r="B335" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C335" s="2">
         <v>211</v>
@@ -12873,7 +12844,7 @@
         <v>2021</v>
       </c>
       <c r="B336" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C336" s="2">
         <v>90</v>
@@ -12908,7 +12879,7 @@
         <v>2021</v>
       </c>
       <c r="B337" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C337" s="2">
         <v>170</v>
@@ -12943,7 +12914,7 @@
         <v>2021</v>
       </c>
       <c r="B338" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C338" s="2">
         <v>1664</v>
@@ -12978,7 +12949,7 @@
         <v>2021</v>
       </c>
       <c r="B339" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C339" s="2">
         <v>1363</v>
@@ -13013,7 +12984,7 @@
         <v>2021</v>
       </c>
       <c r="B340" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C340" s="2">
         <v>162</v>
@@ -13048,7 +13019,7 @@
         <v>2021</v>
       </c>
       <c r="B341" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C341" s="2">
         <v>7</v>
@@ -13083,7 +13054,7 @@
         <v>2021</v>
       </c>
       <c r="B342" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C342" s="2">
         <v>0</v>
@@ -13118,7 +13089,7 @@
         <v>2021</v>
       </c>
       <c r="B343" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C343" s="2">
         <v>0</v>
@@ -13188,7 +13159,7 @@
         <v>2022</v>
       </c>
       <c r="B345" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C345" s="2">
         <v>113</v>
@@ -13223,7 +13194,7 @@
         <v>2022</v>
       </c>
       <c r="B346" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C346" s="2">
         <v>204</v>
@@ -13258,7 +13229,7 @@
         <v>2022</v>
       </c>
       <c r="B347" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C347" s="2">
         <v>42</v>
@@ -13293,7 +13264,7 @@
         <v>2022</v>
       </c>
       <c r="B348" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C348" s="2">
         <v>110</v>
@@ -13328,7 +13299,7 @@
         <v>2022</v>
       </c>
       <c r="B349" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C349" s="2">
         <v>275</v>
@@ -13363,7 +13334,7 @@
         <v>2022</v>
       </c>
       <c r="B350" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C350" s="2">
         <v>350</v>
@@ -13398,7 +13369,7 @@
         <v>2022</v>
       </c>
       <c r="B351" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C351" s="2">
         <v>177</v>
@@ -13433,7 +13404,7 @@
         <v>2022</v>
       </c>
       <c r="B352" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C352" s="2">
         <v>515</v>
@@ -13468,7 +13439,7 @@
         <v>2022</v>
       </c>
       <c r="B353" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C353" s="2">
         <v>1468</v>
@@ -13503,7 +13474,7 @@
         <v>2022</v>
       </c>
       <c r="B354" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C354" s="2">
         <v>159</v>
@@ -13538,7 +13509,7 @@
         <v>2022</v>
       </c>
       <c r="B355" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C355" s="2">
         <v>41</v>
@@ -13573,7 +13544,7 @@
         <v>2022</v>
       </c>
       <c r="B356" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C356" s="2">
         <v>415</v>
@@ -13608,7 +13579,7 @@
         <v>2022</v>
       </c>
       <c r="B357" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C357" s="2">
         <v>320</v>
@@ -13643,7 +13614,7 @@
         <v>2022</v>
       </c>
       <c r="B358" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C358" s="2">
         <v>950</v>
@@ -13678,7 +13649,7 @@
         <v>2022</v>
       </c>
       <c r="B359" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C359" s="2">
         <v>580</v>
@@ -13713,7 +13684,7 @@
         <v>2022</v>
       </c>
       <c r="B360" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C360" s="2">
         <v>168</v>
@@ -13748,7 +13719,7 @@
         <v>2022</v>
       </c>
       <c r="B361" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C361" s="2">
         <v>242</v>
@@ -13783,7 +13754,7 @@
         <v>2022</v>
       </c>
       <c r="B362" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C362" s="2">
         <v>488</v>
@@ -13818,7 +13789,7 @@
         <v>2022</v>
       </c>
       <c r="B363" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C363" s="2">
         <v>163</v>
@@ -13853,7 +13824,7 @@
         <v>2022</v>
       </c>
       <c r="B364" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C364" s="2">
         <v>201</v>
@@ -13888,7 +13859,7 @@
         <v>2022</v>
       </c>
       <c r="B365" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C365" s="2">
         <v>80</v>
@@ -13923,7 +13894,7 @@
         <v>2022</v>
       </c>
       <c r="B366" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C366" s="2">
         <v>157</v>
@@ -13958,7 +13929,7 @@
         <v>2022</v>
       </c>
       <c r="B367" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C367" s="2">
         <v>378</v>
@@ -13993,7 +13964,7 @@
         <v>2022</v>
       </c>
       <c r="B368" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C368" s="2">
         <v>46</v>
@@ -14028,7 +13999,7 @@
         <v>2022</v>
       </c>
       <c r="B369" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C369" s="2">
         <v>145</v>
@@ -14063,7 +14034,7 @@
         <v>2022</v>
       </c>
       <c r="B370" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C370" s="2">
         <v>61</v>
@@ -14098,7 +14069,7 @@
         <v>2022</v>
       </c>
       <c r="B371" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C371" s="2">
         <v>409</v>
@@ -14133,7 +14104,7 @@
         <v>2022</v>
       </c>
       <c r="B372" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C372" s="2">
         <v>546</v>
@@ -14168,7 +14139,7 @@
         <v>2022</v>
       </c>
       <c r="B373" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C373" s="2">
         <v>467</v>
@@ -14203,7 +14174,7 @@
         <v>2022</v>
       </c>
       <c r="B374" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C374" s="2">
         <v>420</v>
@@ -14238,7 +14209,7 @@
         <v>2022</v>
       </c>
       <c r="B375" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C375" s="2">
         <v>71</v>
@@ -14273,7 +14244,7 @@
         <v>2022</v>
       </c>
       <c r="B376" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C376" s="2">
         <v>3142</v>
@@ -14308,7 +14279,7 @@
         <v>2022</v>
       </c>
       <c r="B377" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C377" s="2">
         <v>884</v>
@@ -14343,7 +14314,7 @@
         <v>2022</v>
       </c>
       <c r="B378" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C378" s="2">
         <v>5</v>
@@ -14378,7 +14349,7 @@
         <v>2022</v>
       </c>
       <c r="B379" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C379" s="2">
         <v>170</v>
@@ -14413,7 +14384,7 @@
         <v>2022</v>
       </c>
       <c r="B380" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C380" s="2">
         <v>0</v>
@@ -14448,7 +14419,7 @@
         <v>2022</v>
       </c>
       <c r="B381" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C381" s="2">
         <v>0</v>
@@ -14518,7 +14489,7 @@
         <v>2023</v>
       </c>
       <c r="B383" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C383" s="2">
         <v>2</v>
@@ -14553,7 +14524,7 @@
         <v>2023</v>
       </c>
       <c r="B384" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C384" s="2">
         <v>67</v>
@@ -14588,7 +14559,7 @@
         <v>2023</v>
       </c>
       <c r="B385" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C385" s="2">
         <v>101</v>
@@ -14623,7 +14594,7 @@
         <v>2023</v>
       </c>
       <c r="B386" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C386" s="2">
         <v>179</v>
@@ -14658,7 +14629,7 @@
         <v>2023</v>
       </c>
       <c r="B387" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C387" s="2">
         <v>180</v>
@@ -14693,7 +14664,7 @@
         <v>2023</v>
       </c>
       <c r="B388" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C388" s="2">
         <v>483</v>
@@ -14728,7 +14699,7 @@
         <v>2023</v>
       </c>
       <c r="B389" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C389" s="2">
         <v>333</v>
@@ -14763,7 +14734,7 @@
         <v>2023</v>
       </c>
       <c r="B390" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C390" s="2">
         <v>460</v>
@@ -14798,7 +14769,7 @@
         <v>2023</v>
       </c>
       <c r="B391" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C391" s="2">
         <v>1934</v>
@@ -14833,7 +14804,7 @@
         <v>2023</v>
       </c>
       <c r="B392" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C392" s="2">
         <v>136</v>
@@ -14868,7 +14839,7 @@
         <v>2023</v>
       </c>
       <c r="B393" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C393" s="2">
         <v>50</v>
@@ -14903,7 +14874,7 @@
         <v>2023</v>
       </c>
       <c r="B394" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C394" s="2">
         <v>481</v>
@@ -14938,7 +14909,7 @@
         <v>2023</v>
       </c>
       <c r="B395" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C395" s="2">
         <v>240</v>
@@ -14973,7 +14944,7 @@
         <v>2023</v>
       </c>
       <c r="B396" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C396" s="2">
         <v>971</v>
@@ -15008,7 +14979,7 @@
         <v>2023</v>
       </c>
       <c r="B397" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C397" s="2">
         <v>596</v>
@@ -15043,7 +15014,7 @@
         <v>2023</v>
       </c>
       <c r="B398" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C398" s="2">
         <v>482</v>
@@ -15078,7 +15049,7 @@
         <v>2023</v>
       </c>
       <c r="B399" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C399" s="2">
         <v>160</v>
@@ -15113,7 +15084,7 @@
         <v>2023</v>
       </c>
       <c r="B400" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C400" s="2">
         <v>699</v>
@@ -15148,7 +15119,7 @@
         <v>2023</v>
       </c>
       <c r="B401" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C401" s="2">
         <v>221</v>
@@ -15183,7 +15154,7 @@
         <v>2023</v>
       </c>
       <c r="B402" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C402" s="2">
         <v>317</v>
@@ -15218,7 +15189,7 @@
         <v>2023</v>
       </c>
       <c r="B403" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C403" s="2">
         <v>75</v>
@@ -15253,7 +15224,7 @@
         <v>2023</v>
       </c>
       <c r="B404" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C404" s="2">
         <v>85</v>
@@ -15288,7 +15259,7 @@
         <v>2023</v>
       </c>
       <c r="B405" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C405" s="2">
         <v>495</v>
@@ -15323,7 +15294,7 @@
         <v>2023</v>
       </c>
       <c r="B406" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C406" s="2">
         <v>52</v>
@@ -15358,7 +15329,7 @@
         <v>2023</v>
       </c>
       <c r="B407" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C407" s="2">
         <v>17</v>
@@ -15393,7 +15364,7 @@
         <v>2023</v>
       </c>
       <c r="B408" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C408" s="2">
         <v>91</v>
@@ -15428,7 +15399,7 @@
         <v>2023</v>
       </c>
       <c r="B409" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C409" s="2">
         <v>353</v>
@@ -15463,7 +15434,7 @@
         <v>2023</v>
       </c>
       <c r="B410" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C410" s="2">
         <v>203</v>
@@ -15498,7 +15469,7 @@
         <v>2023</v>
       </c>
       <c r="B411" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C411" s="2">
         <v>570</v>
@@ -15533,7 +15504,7 @@
         <v>2023</v>
       </c>
       <c r="B412" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C412" s="2">
         <v>422</v>
@@ -15568,7 +15539,7 @@
         <v>2023</v>
       </c>
       <c r="B413" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C413" s="2">
         <v>357</v>
@@ -15603,7 +15574,7 @@
         <v>2023</v>
       </c>
       <c r="B414" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C414" s="2">
         <v>3275</v>
@@ -15638,7 +15609,7 @@
         <v>2023</v>
       </c>
       <c r="B415" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C415" s="2">
         <v>646</v>
@@ -15673,7 +15644,7 @@
         <v>2023</v>
       </c>
       <c r="B416" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C416" s="2">
         <v>9</v>
@@ -15708,7 +15679,7 @@
         <v>2023</v>
       </c>
       <c r="B417" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C417" s="2">
         <v>264</v>
@@ -15743,7 +15714,7 @@
         <v>2023</v>
       </c>
       <c r="B418" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C418" s="2">
         <v>0</v>
@@ -15778,7 +15749,7 @@
         <v>2023</v>
       </c>
       <c r="B419" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C419" s="2">
         <v>0</v>
@@ -15883,7 +15854,7 @@
         <v>2024</v>
       </c>
       <c r="B422" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C422" s="2">
         <v>192</v>
@@ -15918,7 +15889,7 @@
         <v>2024</v>
       </c>
       <c r="B423" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C423" s="2">
         <v>69</v>
@@ -15953,7 +15924,7 @@
         <v>2024</v>
       </c>
       <c r="B424" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C424" s="2">
         <v>502</v>
@@ -15988,7 +15959,7 @@
         <v>2024</v>
       </c>
       <c r="B425" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C425" s="2">
         <v>311</v>
@@ -16023,7 +15994,7 @@
         <v>2024</v>
       </c>
       <c r="B426" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C426" s="2">
         <v>170</v>
@@ -16058,7 +16029,7 @@
         <v>2024</v>
       </c>
       <c r="B427" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C427" s="2">
         <v>27</v>
@@ -16093,7 +16064,7 @@
         <v>2024</v>
       </c>
       <c r="B428" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C428" s="2">
         <v>406</v>
@@ -16128,7 +16099,7 @@
         <v>2024</v>
       </c>
       <c r="B429" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C429" s="2">
         <v>88</v>
@@ -16163,7 +16134,7 @@
         <v>2024</v>
       </c>
       <c r="B430" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C430" s="2">
         <v>94</v>
@@ -16198,7 +16169,7 @@
         <v>2024</v>
       </c>
       <c r="B431" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C431" s="2">
         <v>609</v>
@@ -16233,7 +16204,7 @@
         <v>2024</v>
       </c>
       <c r="B432" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C432" s="2">
         <v>297</v>
@@ -16268,7 +16239,7 @@
         <v>2024</v>
       </c>
       <c r="B433" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C433" s="2">
         <v>1480</v>
@@ -16303,7 +16274,7 @@
         <v>2024</v>
       </c>
       <c r="B434" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C434" s="2">
         <v>771</v>
@@ -16338,7 +16309,7 @@
         <v>2024</v>
       </c>
       <c r="B435" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C435" s="2">
         <v>238</v>
@@ -16373,7 +16344,7 @@
         <v>2024</v>
       </c>
       <c r="B436" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C436" s="2">
         <v>393</v>
@@ -16408,7 +16379,7 @@
         <v>2024</v>
       </c>
       <c r="B437" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C437" s="2">
         <v>202</v>
@@ -16443,7 +16414,7 @@
         <v>2024</v>
       </c>
       <c r="B438" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C438" s="2">
         <v>634</v>
@@ -16478,7 +16449,7 @@
         <v>2024</v>
       </c>
       <c r="B439" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C439" s="2">
         <v>260</v>
@@ -16513,7 +16484,7 @@
         <v>2024</v>
       </c>
       <c r="B440" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C440" s="2">
         <v>294</v>
@@ -16548,7 +16519,7 @@
         <v>2024</v>
       </c>
       <c r="B441" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C441" s="2">
         <v>59</v>
@@ -16583,7 +16554,7 @@
         <v>2024</v>
       </c>
       <c r="B442" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C442" s="2">
         <v>177</v>
@@ -16618,7 +16589,7 @@
         <v>2024</v>
       </c>
       <c r="B443" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C443" s="2">
         <v>787</v>
@@ -16653,7 +16624,7 @@
         <v>2024</v>
       </c>
       <c r="B444" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C444" s="2">
         <v>9</v>
@@ -16688,7 +16659,7 @@
         <v>2024</v>
       </c>
       <c r="B445" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C445" s="2">
         <v>5</v>
@@ -16723,7 +16694,7 @@
         <v>2024</v>
       </c>
       <c r="B446" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C446" s="2">
         <v>88</v>
@@ -16758,7 +16729,7 @@
         <v>2024</v>
       </c>
       <c r="B447" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C447" s="2">
         <v>266</v>
@@ -16793,7 +16764,7 @@
         <v>2024</v>
       </c>
       <c r="B448" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C448" s="2">
         <v>162</v>
@@ -16828,7 +16799,7 @@
         <v>2024</v>
       </c>
       <c r="B449" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C449" s="2">
         <v>380</v>
@@ -16863,7 +16834,7 @@
         <v>2024</v>
       </c>
       <c r="B450" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C450" s="2">
         <v>224</v>
@@ -16898,7 +16869,7 @@
         <v>2024</v>
       </c>
       <c r="B451" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C451" s="2">
         <v>3138</v>
@@ -16933,7 +16904,7 @@
         <v>2024</v>
       </c>
       <c r="B452" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C452" s="2">
         <v>117</v>
@@ -16968,7 +16939,7 @@
         <v>2024</v>
       </c>
       <c r="B453" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C453" s="2">
         <v>86</v>
@@ -17003,7 +16974,7 @@
         <v>2024</v>
       </c>
       <c r="B454" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C454" s="2">
         <v>85</v>
@@ -17038,7 +17009,7 @@
         <v>2024</v>
       </c>
       <c r="B455" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C455" s="2">
         <v>214</v>
@@ -17073,7 +17044,7 @@
         <v>2024</v>
       </c>
       <c r="B456" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C456" s="2">
         <v>0</v>
@@ -17108,7 +17079,7 @@
         <v>2024</v>
       </c>
       <c r="B457" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C457" s="2">
         <v>0</v>
@@ -17213,7 +17184,7 @@
         <v>2025</v>
       </c>
       <c r="B460" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C460" s="2">
         <v>85</v>
@@ -17248,7 +17219,7 @@
         <v>2025</v>
       </c>
       <c r="B461" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C461" s="2">
         <v>80</v>
@@ -17283,7 +17254,7 @@
         <v>2025</v>
       </c>
       <c r="B462" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C462" s="2">
         <v>89</v>
@@ -17318,7 +17289,7 @@
         <v>2025</v>
       </c>
       <c r="B463" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C463" s="2">
         <v>110</v>
@@ -17353,7 +17324,7 @@
         <v>2025</v>
       </c>
       <c r="B464" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C464" s="2">
         <v>57</v>
@@ -17388,7 +17359,7 @@
         <v>2025</v>
       </c>
       <c r="B465" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C465" s="2">
         <v>57</v>
@@ -17423,7 +17394,7 @@
         <v>2025</v>
       </c>
       <c r="B466" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C466" s="2">
         <v>137</v>
@@ -17458,7 +17429,7 @@
         <v>2025</v>
       </c>
       <c r="B467" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C467" s="2">
         <v>48</v>
@@ -17493,7 +17464,7 @@
         <v>2025</v>
       </c>
       <c r="B468" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C468" s="2">
         <v>10</v>
@@ -17528,7 +17499,7 @@
         <v>2025</v>
       </c>
       <c r="B469" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C469" s="2">
         <v>96</v>
@@ -17563,7 +17534,7 @@
         <v>2025</v>
       </c>
       <c r="B470" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C470" s="2">
         <v>59</v>
@@ -17598,7 +17569,7 @@
         <v>2025</v>
       </c>
       <c r="B471" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C471" s="2">
         <v>268</v>
@@ -17633,7 +17604,7 @@
         <v>2025</v>
       </c>
       <c r="B472" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C472" s="2">
         <v>171</v>
@@ -17668,7 +17639,7 @@
         <v>2025</v>
       </c>
       <c r="B473" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C473" s="2">
         <v>190</v>
@@ -17703,7 +17674,7 @@
         <v>2025</v>
       </c>
       <c r="B474" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C474" s="2">
         <v>264</v>
@@ -17738,7 +17709,7 @@
         <v>2025</v>
       </c>
       <c r="B475" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C475" s="2">
         <v>78</v>
@@ -17773,7 +17744,7 @@
         <v>2025</v>
       </c>
       <c r="B476" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C476" s="2">
         <v>153</v>
@@ -17808,7 +17779,7 @@
         <v>2025</v>
       </c>
       <c r="B477" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C477" s="2">
         <v>108</v>
@@ -17843,7 +17814,7 @@
         <v>2025</v>
       </c>
       <c r="B478" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C478" s="2">
         <v>33</v>
@@ -17878,7 +17849,7 @@
         <v>2025</v>
       </c>
       <c r="B479" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C479" s="2">
         <v>39</v>
@@ -17913,7 +17884,7 @@
         <v>2025</v>
       </c>
       <c r="B480" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C480" s="2">
         <v>93</v>
@@ -17948,7 +17919,7 @@
         <v>2025</v>
       </c>
       <c r="B481" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C481" s="2">
         <v>0</v>
@@ -17983,7 +17954,7 @@
         <v>2025</v>
       </c>
       <c r="B482" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C482" s="2">
         <v>14</v>
@@ -18018,7 +17989,7 @@
         <v>2025</v>
       </c>
       <c r="B483" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C483" s="2">
         <v>28</v>
@@ -18053,7 +18024,7 @@
         <v>2025</v>
       </c>
       <c r="B484" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C484" s="2">
         <v>57</v>
@@ -18088,7 +18059,7 @@
         <v>2025</v>
       </c>
       <c r="B485" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C485" s="2">
         <v>84</v>
@@ -18123,7 +18094,7 @@
         <v>2025</v>
       </c>
       <c r="B486" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C486" s="2">
         <v>106</v>
@@ -18158,7 +18129,7 @@
         <v>2025</v>
       </c>
       <c r="B487" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C487" s="2">
         <v>27</v>
@@ -18193,7 +18164,7 @@
         <v>2025</v>
       </c>
       <c r="B488" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C488" s="2">
         <v>51</v>
@@ -18228,7 +18199,7 @@
         <v>2025</v>
       </c>
       <c r="B489" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C489" s="2">
         <v>1252</v>
@@ -18263,7 +18234,7 @@
         <v>2025</v>
       </c>
       <c r="B490" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C490" s="2">
         <v>722</v>
@@ -18298,7 +18269,7 @@
         <v>2025</v>
       </c>
       <c r="B491" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C491" s="2">
         <v>127</v>
@@ -18333,7 +18304,7 @@
         <v>2025</v>
       </c>
       <c r="B492" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C492" s="2">
         <v>59</v>
@@ -18368,7 +18339,7 @@
         <v>2025</v>
       </c>
       <c r="B493" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C493" s="2">
         <v>29</v>
@@ -18403,7 +18374,7 @@
         <v>2025</v>
       </c>
       <c r="B494" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C494" s="2">
         <v>0</v>
@@ -18438,7 +18409,7 @@
         <v>2025</v>
       </c>
       <c r="B495" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C495" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
refactor: Cambio de nombre a encabezados de algunas columnas
</commit_message>
<xml_diff>
--- a/data/processed/servicios_cult_soc_dep_rec_issste2025.xlsx
+++ b/data/processed/servicios_cult_soc_dep_rec_issste2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA7BBC6-4E14-467B-B2FA-161BA24971B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0E1F07-7A2F-405D-A314-7A5E721BDE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="3" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
@@ -208,13 +208,7 @@
     <t>Subdelegación. Poniente</t>
   </si>
   <si>
-    <t>Etiquetas de fila</t>
-  </si>
-  <si>
     <t>Total general</t>
-  </si>
-  <si>
-    <t>Etiquetas de columna</t>
   </si>
   <si>
     <t>Suma de Serv. Deportivos Derecho Hab Publ</t>
@@ -244,7 +238,13 @@
     <t>Suma de todos los Servicios</t>
   </si>
   <si>
-    <t>Suma de Suma de todos los Servicios</t>
+    <t>Años</t>
+  </si>
+  <si>
+    <t>Nombre Oficina Representación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suma de todos los Servicios </t>
   </si>
 </sst>
 </file>
@@ -10012,7 +10012,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
   <location ref="A4:AY19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="1" showAll="0">
@@ -10316,7 +10316,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A4:I54" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -10592,7 +10592,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A7:B57" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -12988,7 +12988,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Suma de Suma de todos los Servicios" fld="11" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Suma de todos los Servicios " fld="11" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -13328,7 +13328,7 @@
   <dimension ref="A1:L495"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13382,7 +13382,7 @@
         <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -32664,13 +32664,13 @@
   <dimension ref="A4:AY19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
@@ -32724,15 +32724,15 @@
   <sheetData>
     <row r="4" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -32882,7 +32882,7 @@
         <v>23</v>
       </c>
       <c r="AY5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.3">
@@ -34616,7 +34616,7 @@
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2">
         <v>160650</v>
@@ -34779,12 +34779,12 @@
   <dimension ref="A4:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
@@ -34797,31 +34797,31 @@
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>65</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>66</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>67</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -36247,7 +36247,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" s="2">
         <v>36375442</v>
@@ -36284,7 +36284,7 @@
   <dimension ref="A7:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36738,7 +36738,7 @@
   <sheetData>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
@@ -37138,7 +37138,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="2">
         <v>56915689</v>

</xml_diff>